<commit_message>
fix data version used
</commit_message>
<xml_diff>
--- a/Reproducibility Package/documentation/rider-audits/pooled/codebooks/label-constructed-data.xlsx
+++ b/Reproducibility Package/documentation/rider-audits/pooled/codebooks/label-constructed-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wb501238\Documents\GitHub\rio-safe-space\Reproducibility Package\documentation\rider-audits\pooled\codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luizaandrade\Documents\GitHub\rio-safe-space\Reproducibility Package\documentation\rider-audits\pooled\codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A192EA74-C406-4155-AB98-17D1C18D538F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C00418C-0778-417F-9AE3-13CE6F85CA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="21864" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2788" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2789" uniqueCount="762">
   <si>
     <t>name</t>
   </si>
@@ -2672,16 +2672,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I346"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="E125" sqref="E125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="68.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -2850,6 +2850,9 @@
       </c>
     </row>
     <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
       <c r="B7" t="s">
         <v>657</v>
       </c>
@@ -11571,9 +11574,9 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11841,7 +11844,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">

</xml_diff>